<commit_message>
Update RRLS Pedals Hardware BOM for v204.xlsx
Included pricing from one possible source. (Fastenal)
Pricing is not complete.
</commit_message>
<xml_diff>
--- a/RRLS Pedals Hardware BOM for v204.xlsx
+++ b/RRLS Pedals Hardware BOM for v204.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\3D Printing\STLs\Flight Sim Parts\RRLS_Printed Parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430F90EF-4F2C-4BB9-9993-3F64E1DCA381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A17133-7212-4A28-9554-5B3E090BEC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19515" yWindow="900" windowWidth="19260" windowHeight="14370" xr2:uid="{22EF5506-1B59-476C-B271-3B72D4B35AAE}"/>
+    <workbookView xWindow="-28920" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{22EF5506-1B59-476C-B271-3B72D4B35AAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,22 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="102">
   <si>
     <t>Bolts</t>
   </si>
@@ -166,9 +156,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Drawing shows shoulder bolts but nut placement require all-thread</t>
-  </si>
-  <si>
     <t>Counted anywhere bolt terminated in extrusion</t>
   </si>
   <si>
@@ -241,9 +228,6 @@
     <t>92010A328_NO THREADS_Passivated 18-8 stainless Steel Phillips Flat Head Screw</t>
   </si>
   <si>
-    <t>Airline Pedal Version Only</t>
-  </si>
-  <si>
     <t>Does not include 4 608 bearings in toe brake add-on</t>
   </si>
   <si>
@@ -277,13 +261,76 @@
     <t>Version 204 BOM</t>
   </si>
   <si>
-    <t>(Distributed with cost section left blank due to significant variation in cost and availability of parts based on region)</t>
-  </si>
-  <si>
     <t>2020 Extrusion lengths</t>
   </si>
   <si>
     <t>Still in development. No hardware for mounting listed in this version of BOM</t>
+  </si>
+  <si>
+    <t>Sold As</t>
+  </si>
+  <si>
+    <t>Order Qty</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>ea</t>
+  </si>
+  <si>
+    <t>https://www.fastenal.com/product/details/11103212#</t>
+  </si>
+  <si>
+    <t>https://www.fastenal.com/product/details/11103206#</t>
+  </si>
+  <si>
+    <t>https://www.fastenal.com/product/details/ZS2540016ZP0000#</t>
+  </si>
+  <si>
+    <t>https://www.fastenal.com/product/details/0121814#</t>
+  </si>
+  <si>
+    <t>Drawing shows shoulder bolts but nut placement requires all-thread. Swapped to hex head</t>
+  </si>
+  <si>
+    <t>https://www.fastenal.com/product/details/ZS2530020ZP0000#</t>
+  </si>
+  <si>
+    <t>https://www.fastenal.com/product/details/MS2540050A20000#</t>
+  </si>
+  <si>
+    <t>https://www.fastenal.com/product/details/11113827#</t>
+  </si>
+  <si>
+    <t>Selected hex head bolt</t>
+  </si>
+  <si>
+    <t>https://www.fastenal.com/product/details/ZS2580035ZP0000#</t>
+  </si>
+  <si>
+    <t>https://www.fastenal.com/product/details/ZS2550025ZP0000#</t>
+  </si>
+  <si>
+    <t>https://www.fastenal.com/product/details/1L2580000A40000#</t>
+  </si>
+  <si>
+    <t>https://www.fastenal.com/product/details/1L2540000A40000#</t>
+  </si>
+  <si>
+    <t>https://www.fastenal.com/product/details/40252#</t>
+  </si>
+  <si>
+    <t>Amazon (for return policy)</t>
+  </si>
+  <si>
+    <t>https://www.fastenal.com/product/details/MW6380000A40000#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Airline Pedal Version Only. No source. Can't find reasonably priced source (didn't try very hard) </t>
+  </si>
+  <si>
+    <t>pricing sourced from Fastenal in US as many bolts can be purchased individually.  Cheaper sources can be found especially if buying in bulk</t>
   </si>
 </sst>
 </file>
@@ -293,7 +340,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,6 +358,14 @@
     <font>
       <sz val="11"/>
       <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -345,15 +400,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -366,11 +421,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -683,42 +740,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A2194C-9C13-4484-AFB6-E8121AF71D28}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="50.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="62.7109375" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="57.42578125" customWidth="1"/>
+    <col min="9" max="9" width="62.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="10">
-        <f>SUM(E4,E6,E8,E18,E21,E26,E35,E42,E45,)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="9">
+        <f>SUM(G4,G6,G8,G18,G21,G26,G35,G42,G45,)</f>
+        <v>37.710100000000004</v>
+      </c>
+      <c r="H1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -729,80 +790,95 @@
         <v>34</v>
       </c>
       <c r="D3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" t="s">
         <v>38</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="H3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="9">
-        <f>SUM(E5)</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="8">
+        <f>SUM(G5)</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="9">
-        <f>SUM(E7)</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="8">
+        <f>SUM(G7)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="I7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="9">
-        <f>SUM(E9:E17)</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="8">
+        <f>SUM(G9:G17)</f>
+        <v>16.220800000000001</v>
+      </c>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -812,16 +888,24 @@
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <f>D54</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.1285</v>
+      </c>
+      <c r="G9" s="3">
+        <f>F9*E9</f>
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -831,16 +915,24 @@
       <c r="C10" s="2">
         <v>5</v>
       </c>
-      <c r="D10" s="5">
-        <v>0</v>
-      </c>
-      <c r="E10" s="5">
-        <f>D64</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="4">
+        <v>8.5099999999999995E-2</v>
+      </c>
+      <c r="G10" s="4">
+        <f>F10*E10</f>
+        <v>0.42549999999999999</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -850,16 +942,24 @@
       <c r="C11">
         <v>21</v>
       </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <f>D65</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11">
+        <v>21</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.1033</v>
+      </c>
+      <c r="G11" s="6">
+        <f t="shared" ref="G11:G17" si="0">F11*E11</f>
+        <v>2.1693000000000002</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -869,18 +969,27 @@
       <c r="C12" s="2">
         <v>2</v>
       </c>
-      <c r="D12" s="5">
-        <v>0</v>
-      </c>
-      <c r="E12" s="5">
-        <f>D66</f>
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.54959999999999998</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0992</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -890,15 +999,24 @@
       <c r="C13">
         <v>19</v>
       </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-      <c r="E13" s="4">
-        <f>D67</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13">
+        <v>19</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.11360000000000001</v>
+      </c>
+      <c r="G13" s="6">
+        <f t="shared" si="0"/>
+        <v>2.1584000000000003</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -908,15 +1026,24 @@
       <c r="C14" s="2">
         <v>10</v>
       </c>
-      <c r="D14" s="5">
-        <v>0</v>
-      </c>
-      <c r="E14" s="5">
-        <f>D68</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="2">
+        <v>10</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.48170000000000002</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="0"/>
+        <v>4.8170000000000002</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -926,15 +1053,24 @@
       <c r="C15">
         <v>4</v>
       </c>
-      <c r="D15" s="4">
-        <v>0</v>
-      </c>
-      <c r="E15" s="4">
-        <f>D69</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.48870000000000002</v>
+      </c>
+      <c r="G15" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9548000000000001</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="I15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -944,15 +1080,22 @@
       <c r="C16" s="2">
         <v>6</v>
       </c>
-      <c r="D16" s="5">
-        <v>0</v>
-      </c>
-      <c r="E16" s="5">
-        <f>D70</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2">
+        <v>6</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.43359999999999999</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="0"/>
+        <v>2.6015999999999999</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -962,29 +1105,38 @@
       <c r="C17">
         <v>4</v>
       </c>
-      <c r="D17" s="4">
-        <v>0</v>
-      </c>
-      <c r="E17" s="4">
-        <f>D71</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.1845</v>
+      </c>
+      <c r="G17" s="6">
+        <f t="shared" si="0"/>
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="6">
-        <f>SUM(E19:E20)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="5">
+        <f>SUM(G19:G20)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -994,18 +1146,24 @@
       <c r="C19">
         <v>16</v>
       </c>
-      <c r="D19" s="4">
-        <v>0</v>
-      </c>
-      <c r="E19" s="4">
-        <f>D73</f>
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>16</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <f>F73</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
@@ -1015,29 +1173,39 @@
       <c r="C20" s="2">
         <v>2</v>
       </c>
-      <c r="D20" s="5">
-        <v>0</v>
-      </c>
-      <c r="E20" s="5">
-        <f>D74</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="2"/>
+      <c r="E20" s="2">
+        <v>2</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
+        <f>F74</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="6">
-        <f>SUM(E22:E25)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="5">
+        <f>SUM(G22:G25)</f>
+        <v>4.1105999999999998</v>
+      </c>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1047,15 +1215,21 @@
       <c r="C22">
         <v>4</v>
       </c>
-      <c r="D22" s="4">
-        <v>0</v>
-      </c>
-      <c r="E22" s="4">
-        <f>D76</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.59109999999999996</v>
+      </c>
+      <c r="G22" s="3">
+        <f>F22*E22</f>
+        <v>2.3643999999999998</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -1065,15 +1239,22 @@
       <c r="C23" s="2">
         <v>10</v>
       </c>
-      <c r="D23" s="5">
-        <v>0</v>
-      </c>
-      <c r="E23" s="5">
-        <f>D77</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2">
+        <v>10</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0.16320000000000001</v>
+      </c>
+      <c r="G23" s="4">
+        <f>F23*E23</f>
+        <v>1.6320000000000001</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1083,15 +1264,21 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" s="4">
-        <v>0</v>
-      </c>
-      <c r="E24" s="4">
-        <f>D78</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24" s="3">
+        <v>5.7099999999999998E-2</v>
+      </c>
+      <c r="G24" s="3">
+        <f>F24*E24</f>
+        <v>0.1142</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>36</v>
       </c>
@@ -1101,56 +1288,72 @@
       <c r="C25" s="2">
         <v>21</v>
       </c>
-      <c r="D25" s="5">
-        <v>0</v>
-      </c>
-      <c r="E25" s="5">
-        <f>D79</f>
-        <v>0</v>
-      </c>
-      <c r="F25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2">
+        <v>21</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25" s="4">
+        <f>F25*E25</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="6">
-        <f>SUM(E27:E36)</f>
-        <v>0</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="G26" s="5">
+        <f>SUM(G27:G36)</f>
+        <v>12.791600000000001</v>
+      </c>
+      <c r="H26" s="5"/>
+      <c r="I26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27" s="6">
+        <v>0</v>
+      </c>
+      <c r="G27" s="6">
+        <f>F27*E27</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="I27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="3">
-        <v>4</v>
-      </c>
-      <c r="D27" s="7">
-        <v>0</v>
-      </c>
-      <c r="E27" s="7">
-        <f>D27*C27</f>
-        <v>0</v>
-      </c>
-      <c r="F27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
@@ -1160,81 +1363,105 @@
       <c r="C28" s="2">
         <v>4</v>
       </c>
-      <c r="D28" s="5">
-        <v>0</v>
-      </c>
-      <c r="E28" s="5">
-        <f t="shared" ref="E28:E31" si="0">D28*C28</f>
-        <v>0</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="D28" s="2"/>
+      <c r="E28" s="2">
+        <v>4</v>
+      </c>
+      <c r="F28" s="4">
+        <v>0.43359999999999999</v>
+      </c>
+      <c r="G28" s="4">
+        <f>F28*E28</f>
+        <v>1.7343999999999999</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <v>16</v>
+      </c>
+      <c r="E29">
+        <v>16</v>
+      </c>
+      <c r="F29" s="6">
+        <v>0.11360000000000001</v>
+      </c>
+      <c r="G29" s="6">
+        <f>F29*E29</f>
+        <v>1.8176000000000001</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="3">
-        <v>16</v>
-      </c>
-      <c r="D29" s="7">
-        <v>0</v>
-      </c>
-      <c r="E29" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="C30" s="2">
         <v>2</v>
       </c>
-      <c r="D30" s="5">
-        <v>0</v>
-      </c>
-      <c r="E30" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F30" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="D30" s="2"/>
+      <c r="E30" s="2">
+        <v>2</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0</v>
+      </c>
+      <c r="G30" s="4">
+        <f>F30*E30</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="4"/>
+      <c r="I30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="3">
+      <c r="C31">
         <v>2</v>
       </c>
-      <c r="D31" s="7">
-        <v>0</v>
-      </c>
-      <c r="E31" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F31" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31" s="6">
+        <v>0.1066</v>
+      </c>
+      <c r="G31" s="6">
+        <f>F31*E31</f>
+        <v>0.2132</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
@@ -1244,74 +1471,93 @@
       <c r="C32" s="2">
         <v>10</v>
       </c>
-      <c r="D32" s="5">
-        <v>0</v>
-      </c>
-      <c r="E32" s="5">
-        <f t="shared" ref="E32" si="1">D32*C32</f>
-        <v>0</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="D32" s="2"/>
+      <c r="E32" s="2">
+        <v>10</v>
+      </c>
+      <c r="F32" s="4">
+        <v>0.43359999999999999</v>
+      </c>
+      <c r="G32" s="4">
+        <f>F32*E32</f>
+        <v>4.3360000000000003</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="B33" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" s="3">
+      <c r="C33">
         <v>6</v>
       </c>
-      <c r="D33" s="7">
-        <v>0</v>
-      </c>
-      <c r="E33" s="7">
-        <f t="shared" ref="E33:E34" si="2">D33*C33</f>
-        <v>0</v>
-      </c>
-      <c r="F33" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>6</v>
+      </c>
+      <c r="F33" s="6">
+        <v>0</v>
+      </c>
+      <c r="G33" s="6">
+        <f>F33*E33</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C34" s="2">
         <v>2</v>
       </c>
-      <c r="D34" s="5">
-        <v>0</v>
-      </c>
-      <c r="E34" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F34" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D34" s="2"/>
+      <c r="E34" s="2">
+        <v>2</v>
+      </c>
+      <c r="F34" s="4">
+        <v>0</v>
+      </c>
+      <c r="G34" s="4">
+        <f>F34*E34</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="4"/>
+      <c r="I34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E35" s="6">
-        <f>SUM(E36:E40)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="5">
+        <f>SUM(G36:G40)</f>
+        <v>4.5870999999999995</v>
+      </c>
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1321,15 +1567,21 @@
       <c r="C36">
         <v>1</v>
       </c>
-      <c r="D36" s="4">
-        <v>0</v>
-      </c>
-      <c r="E36" s="4">
-        <f>D81</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0.1033</v>
+      </c>
+      <c r="G36" s="3">
+        <f>F36*E36</f>
+        <v>0.1033</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>6</v>
       </c>
@@ -1339,15 +1591,22 @@
       <c r="C37" s="2">
         <v>4</v>
       </c>
-      <c r="D37" s="5">
-        <v>0</v>
-      </c>
-      <c r="E37" s="5">
-        <f>D82</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D37" s="2"/>
+      <c r="E37" s="2">
+        <v>4</v>
+      </c>
+      <c r="F37" s="4">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="G37" s="4">
+        <f>F37*E37</f>
+        <v>3.4039999999999999</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -1357,15 +1616,21 @@
       <c r="C38">
         <v>1</v>
       </c>
-      <c r="D38" s="4">
-        <v>0</v>
-      </c>
-      <c r="E38" s="4">
-        <f>D83</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0.59109999999999996</v>
+      </c>
+      <c r="G38" s="3">
+        <f>F38*E38</f>
+        <v>0.59109999999999996</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>18</v>
       </c>
@@ -1375,89 +1640,116 @@
       <c r="C39" s="2">
         <v>1</v>
       </c>
-      <c r="D39" s="5">
-        <v>0</v>
-      </c>
-      <c r="E39" s="5">
-        <f>D84</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="D39" s="2"/>
+      <c r="E39" s="2">
+        <v>1</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0.48870000000000002</v>
+      </c>
+      <c r="G39" s="4">
+        <f>F39*E39</f>
+        <v>0.48870000000000002</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40">
         <v>4</v>
       </c>
-      <c r="D40" s="7">
-        <v>0</v>
-      </c>
-      <c r="E40" s="7">
-        <f>D85</f>
-        <v>0</v>
-      </c>
-      <c r="F40" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40" s="6">
+        <v>0</v>
+      </c>
+      <c r="G40" s="6">
+        <f t="shared" ref="G36:G41" si="1">F85</f>
+        <v>0</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="I40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C41" s="2">
         <v>1</v>
       </c>
-      <c r="D41" s="5">
-        <v>0</v>
-      </c>
-      <c r="E41" s="5">
-        <f>D86</f>
-        <v>0</v>
-      </c>
-      <c r="F41" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D41" s="2"/>
+      <c r="E41" s="2">
+        <v>1</v>
+      </c>
+      <c r="F41" s="4">
+        <v>0</v>
+      </c>
+      <c r="G41" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I41" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E42" s="6">
-        <f>SUM(E43:E44)</f>
-        <v>0</v>
-      </c>
-      <c r="F42" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="5">
+        <f>SUM(G43:G44)</f>
+        <v>0</v>
+      </c>
+      <c r="H42" s="5"/>
+      <c r="I42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>32</v>
       </c>
       <c r="C43">
         <v>3</v>
       </c>
-      <c r="D43" s="4">
-        <v>0</v>
-      </c>
-      <c r="E43" s="4">
-        <f t="shared" ref="E43:E44" si="3">D87</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0</v>
+      </c>
+      <c r="G43" s="3">
+        <f t="shared" ref="G43:G44" si="2">F87</f>
+        <v>0</v>
+      </c>
+      <c r="H43" s="3"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>33</v>
       </c>
@@ -1465,86 +1757,113 @@
       <c r="C44" s="2">
         <v>2</v>
       </c>
-      <c r="D44" s="5">
-        <v>0</v>
-      </c>
-      <c r="E44" s="5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D44" s="2"/>
+      <c r="E44" s="2">
+        <v>2</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0</v>
+      </c>
+      <c r="G44" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E45" s="6">
-        <f>SUM(E46:E48)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="5">
+        <f>SUM(G46:G48)</f>
+        <v>0</v>
+      </c>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46">
         <v>2</v>
       </c>
-      <c r="D46" s="4">
-        <v>0</v>
-      </c>
-      <c r="E46" s="10">
-        <f>D46*C46</f>
-        <v>0</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46" s="3">
+        <v>0</v>
+      </c>
+      <c r="G46" s="9">
+        <f>F46*E46</f>
+        <v>0</v>
+      </c>
+      <c r="H46" s="9"/>
+      <c r="I46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C47" s="2">
         <v>4</v>
       </c>
-      <c r="D47" s="5">
-        <v>0</v>
-      </c>
-      <c r="E47" s="5">
-        <f>D47*C47</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D47" s="2"/>
+      <c r="E47" s="2">
+        <v>4</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0</v>
+      </c>
+      <c r="G47" s="4">
+        <f>F47*E47</f>
+        <v>0</v>
+      </c>
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
-      <c r="D48" s="7">
-        <v>0</v>
-      </c>
-      <c r="E48" s="7">
-        <f>D48*C48</f>
-        <v>0</v>
-      </c>
-      <c r="F48" t="s">
-        <v>70</v>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="6">
+        <v>0</v>
+      </c>
+      <c r="G48" s="6">
+        <f>F48*E48</f>
+        <v>0</v>
+      </c>
+      <c r="H48" s="6"/>
+      <c r="I48" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H16" r:id="rId1" xr:uid="{FFD0BCE9-FF26-4281-886B-15F64C835CE2}"/>
+    <hyperlink ref="H13" r:id="rId2" xr:uid="{8630D227-FBD6-4358-B75B-3952927D3883}"/>
+    <hyperlink ref="H11" r:id="rId3" xr:uid="{5A494CEF-4D18-4F72-8F8F-75F9591FFC37}"/>
+    <hyperlink ref="H15" r:id="rId4" xr:uid="{EF70BC7A-DCC7-4609-9E06-C648D14A4323}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>